<commit_message>
fix salary import data
</commit_message>
<xml_diff>
--- a/QMPlusServer/static/template/salarys.xlsx
+++ b/QMPlusServer/static/template/salarys.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -173,6 +173,14 @@
   </si>
   <si>
     <t>总经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司名称(与录入数据库名称一致)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿里</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -510,191 +518,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="7.75" customWidth="1"/>
-    <col min="4" max="4" width="5.75" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="9.875" customWidth="1"/>
-    <col min="7" max="7" width="11.375" customWidth="1"/>
-    <col min="8" max="9" width="9.125" customWidth="1"/>
-    <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="15.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="8.875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="30.25" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="7.75" customWidth="1"/>
+    <col min="5" max="5" width="5.75" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="9.875" customWidth="1"/>
+    <col min="8" max="8" width="11.375" customWidth="1"/>
+    <col min="9" max="10" width="9.125" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="15.25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.625" style="1" customWidth="1"/>
+    <col min="16" max="17" width="8.875" style="1" customWidth="1"/>
+    <col min="28" max="28" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2020</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>38</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2000</v>
-      </c>
-      <c r="G2">
-        <v>1000</v>
       </c>
       <c r="H2">
         <v>1000</v>
       </c>
       <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
         <v>0.3</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>1000</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1100</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>0</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>10</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>5</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -706,21 +718,24 @@
         <v>0</v>
       </c>
       <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
         <v>10000</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>9350</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>700</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>1200</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>2000</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>8900</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tmplate add ten attr
</commit_message>
<xml_diff>
--- a/QMPlusServer/static/template/salarys.xlsx
+++ b/QMPlusServer/static/template/salarys.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,6 +181,46 @@
   </si>
   <si>
     <t>张三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ext10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -518,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AQ2" sqref="AQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -543,7 +583,7 @@
     <col min="29" max="29" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -643,8 +683,38 @@
       <c r="AG1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="AH1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -743,6 +813,36 @@
       </c>
       <c r="AG2">
         <v>8900</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>